<commit_message>
Add support for delimited file export
</commit_message>
<xml_diff>
--- a/src/main/resources/com/cmc/testing/filetester/template.xlsx
+++ b/src/main/resources/com/cmc/testing/filetester/template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhogan/dev/file-tester/src/main/resources/com/cmc/testing/filetester/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>First Name</t>
   </si>
@@ -56,6 +61,30 @@
   </si>
   <si>
     <t>Field Name</t>
+  </si>
+  <si>
+    <t>Fixed Length</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>TAB</t>
+  </si>
+  <si>
+    <t>Export Type</t>
+  </si>
+  <si>
+    <t>Delimiter</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -112,18 +141,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -449,58 +484,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="4" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="16" width="10.83203125" style="4"/>
+    <col min="17" max="17" width="18.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="R4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B5" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="R5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B6" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2">
+      <formula1>"Fixed Length,Delimited"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>$R$1:$R$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -512,9 +586,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -536,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -547,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -560,10 +634,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pipe character to the delimieter list.
</commit_message>
<xml_diff>
--- a/src/main/resources/com/cmc/testing/filetester/template.xlsx
+++ b/src/main/resources/com/cmc/testing/filetester/template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -555,6 +558,9 @@
       <c r="B6" s="4">
         <v>20</v>
       </c>
+      <c r="R6" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -570,7 +576,7 @@
       <formula1>"Fixed Length,Delimited"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>$R$1:$R$5</formula1>
+      <formula1>$R$1:$R$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>